<commit_message>
Testing of latitude/longitude coordinates
</commit_message>
<xml_diff>
--- a/track-map/ConePositions.xlsx
+++ b/track-map/ConePositions.xlsx
@@ -28,7 +28,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -38,14 +38,16 @@
     </border>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60,14 +62,14 @@
   <cols>
     <col min="1" max="1" width="11.60546875" customWidth="true"/>
     <col min="2" max="2" width="11.60546875" customWidth="true"/>
-    <col min="3" max="3" width="11.60546875" customWidth="true"/>
+    <col min="3" max="3" width="10.60546875" customWidth="true"/>
     <col min="4" max="4" width="11.60546875" customWidth="true"/>
-    <col min="5" max="5" width="10.60546875" customWidth="true"/>
+    <col min="5" max="5" width="11.60546875" customWidth="true"/>
     <col min="6" max="6" width="11.60546875" customWidth="true"/>
     <col min="7" max="7" width="11.60546875" customWidth="true"/>
     <col min="8" max="8" width="11.60546875" customWidth="true"/>
     <col min="9" max="9" width="11.60546875" customWidth="true"/>
-    <col min="10" max="10" width="10.60546875" customWidth="true"/>
+    <col min="10" max="10" width="11.60546875" customWidth="true"/>
     <col min="11" max="11" width="11.60546875" customWidth="true"/>
     <col min="12" max="12" width="11.60546875" customWidth="true"/>
     <col min="13" max="13" width="11.60546875" customWidth="true"/>
@@ -121,40 +123,40 @@
         <v>33.778086278122842</v>
       </c>
       <c r="B1" s="0">
-        <v>33.778084552795036</v>
+        <v>33.777816264320222</v>
       </c>
       <c r="C1" s="0">
-        <v>33.777816264320222</v>
+        <v>33.777665298136647</v>
       </c>
       <c r="D1" s="0">
-        <v>33.777814538992409</v>
+        <v>33.777548838509318</v>
       </c>
       <c r="E1" s="0">
-        <v>33.777665298136647</v>
+        <v>33.777930135955835</v>
       </c>
       <c r="F1" s="0">
-        <v>33.777663572808834</v>
+        <v>33.778154428571433</v>
       </c>
       <c r="G1" s="0">
-        <v>33.777548838509318</v>
+        <v>33.778037106280195</v>
       </c>
       <c r="H1" s="0">
-        <v>33.777930135955835</v>
+        <v>33.777945663906145</v>
       </c>
       <c r="I1" s="0">
-        <v>33.778154428571433</v>
+        <v>33.777967230503798</v>
       </c>
       <c r="J1" s="0">
-        <v>33.77815270324362</v>
+        <v>33.777641143547271</v>
       </c>
       <c r="K1" s="0">
-        <v>33.778150977915807</v>
+        <v>33.777637692891652</v>
       </c>
       <c r="L1" s="0">
-        <v>33.778037106280195</v>
+        <v>33.778091454106281</v>
       </c>
       <c r="M1" s="0">
-        <v>33.778035380952382</v>
+        <v>33.777843006901314</v>
       </c>
       <c r="N1" s="0">
         <v>33.777945663906145</v>
@@ -291,40 +293,40 @@
         <v>-84.399651332089547</v>
       </c>
       <c r="B2" s="0">
-        <v>-84.39965237313433</v>
+        <v>-84.399669029850742</v>
       </c>
       <c r="C2" s="0">
-        <v>-84.399669029850742</v>
+        <v>-84.399711712686567</v>
       </c>
       <c r="D2" s="0">
-        <v>-84.399671111940293</v>
+        <v>-84.39976480597015</v>
       </c>
       <c r="E2" s="0">
-        <v>-84.399711712686567</v>
+        <v>-84.39977938059701</v>
       </c>
       <c r="F2" s="0">
-        <v>-84.399712753731336</v>
+        <v>-84.399801242537308</v>
       </c>
       <c r="G2" s="0">
-        <v>-84.39976480597015</v>
+        <v>-84.39981373507463</v>
       </c>
       <c r="H2" s="0">
-        <v>-84.39977938059701</v>
+        <v>-84.399894936567165</v>
       </c>
       <c r="I2" s="0">
-        <v>-84.399801242537308</v>
+        <v>-84.399916798507462</v>
       </c>
       <c r="J2" s="0">
-        <v>-84.39980228358209</v>
+        <v>-84.399946988805965</v>
       </c>
       <c r="K2" s="0">
-        <v>-84.399803324626859</v>
+        <v>-84.399948029850748</v>
       </c>
       <c r="L2" s="0">
-        <v>-84.39981373507463</v>
+        <v>-84.400020902985077</v>
       </c>
       <c r="M2" s="0">
-        <v>-84.399814776119399</v>
+        <v>-84.400054216417914</v>
       </c>
       <c r="N2" s="0">
         <v>-84.399894936567165</v>

</xml_diff>

<commit_message>
Added a better verification system + started on grouping
</commit_message>
<xml_diff>
--- a/track-map/ConePositions.xlsx
+++ b/track-map/ConePositions.xlsx
@@ -28,7 +28,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -39,15 +39,35 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
Fixed bad excel outputs
</commit_message>
<xml_diff>
--- a/track-map/ConePositions.xlsx
+++ b/track-map/ConePositions.xlsx
@@ -111,26 +111,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>33.777551857832989</v>
-      </c>
-      <c r="B1" s="0">
-        <v>-84.399772613805965</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>33.777641143547271</v>
-      </c>
-      <c r="B2" s="0">
-        <v>-84.399946988805965</v>
+        <v>33.777666592132505</v>
+      </c>
+      <c r="B1" s="0">
+        <v>-84.399718479477613</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>33.777818852311938</v>
+      </c>
+      <c r="B2" s="0">
+        <v>-84.399675796641787</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>33.777641143547271</v>
+        <v>33.777845163561075</v>
       </c>
       <c r="B3" s="0">
-        <v>-84.399954796641794</v>
+        <v>-84.400060983208945</v>
       </c>
     </row>
   </sheetData>
@@ -148,26 +148,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>33.777551857832989</v>
-      </c>
-      <c r="B1" s="0">
-        <v>-84.399772613805965</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>33.777641143547271</v>
-      </c>
-      <c r="B2" s="0">
-        <v>-84.399946988805965</v>
+        <v>33.777932292615596</v>
+      </c>
+      <c r="B1" s="0">
+        <v>-84.399786147388056</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>33.777948251897861</v>
+      </c>
+      <c r="B2" s="0">
+        <v>-84.399901703358211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>33.777641143547271</v>
+        <v>33.777968093167701</v>
       </c>
       <c r="B3" s="0">
-        <v>-84.399954796641794</v>
+        <v>-84.399924085820899</v>
       </c>
     </row>
   </sheetData>
@@ -176,35 +176,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.60546875" customWidth="true"/>
-    <col min="2" max="2" width="12.1875" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0">
-        <v>33.777551857832989</v>
-      </c>
-      <c r="B1" s="0">
-        <v>-84.399772613805965</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>33.777641143547271</v>
-      </c>
-      <c r="B2" s="0">
-        <v>-84.399946988805965</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>33.777641143547271</v>
-      </c>
-      <c r="B3" s="0">
-        <v>-84.399954796641794</v>
+  <dimension ref="A1:B2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.60546875" customWidth="true"/>
+    <col min="2" max="2" width="11.1875" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0">
+        <v>33.778039262939963</v>
+      </c>
+      <c r="B1" s="0">
+        <v>-84.399820501865662</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>33.778087572118707</v>
+      </c>
+      <c r="B2" s="0">
+        <v>-84.399658098880593</v>
       </c>
     </row>
   </sheetData>
@@ -213,35 +205,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.60546875" customWidth="true"/>
-    <col min="2" max="2" width="12.1875" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0">
-        <v>33.777551857832989</v>
-      </c>
-      <c r="B1" s="0">
-        <v>-84.399772613805965</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>33.777641143547271</v>
-      </c>
-      <c r="B2" s="0">
-        <v>-84.399946988805965</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>33.777641143547271</v>
-      </c>
-      <c r="B3" s="0">
-        <v>-84.399954796641794</v>
+  <dimension ref="A1:B2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.60546875" customWidth="true"/>
+    <col min="2" max="2" width="12.1875" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0">
+        <v>33.778094042098004</v>
+      </c>
+      <c r="B1" s="0">
+        <v>-84.400027149253731</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>33.778155291235336</v>
+      </c>
+      <c r="B2" s="0">
+        <v>-84.399808009328353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>